<commit_message>
Final Testing and Documentation
</commit_message>
<xml_diff>
--- a/Project 3 Test Plan.xlsx
+++ b/Project 3 Test Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chevy\Desktop\CIS 435\CIS435-Project3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c6b9c66a2bd56c32/Programming/Project 3/CIS435-Project3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52570753-5CC9-4F1E-9A05-319F2D7CD941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{52570753-5CC9-4F1E-9A05-319F2D7CD941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CC8BBA1-F9CF-4EA0-AED6-D4E1DBC76C5B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="November 19, 2021" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="75">
   <si>
     <t>#</t>
   </si>
@@ -222,9 +222,6 @@
     <t>When the Remove Note button is clicked with one or more checkboxes checked, the corresponding notes for each checkbox are deleted from the username.txt file on the back end, and the list view is updated to show only the remaining notes, a message is alsxo displayed confirming the notes were successfully deleted</t>
   </si>
   <si>
-    <t>Test case plan - Day 4 (Final Bug Testing and Word Counter)</t>
-  </si>
-  <si>
     <t>Chevy</t>
   </si>
   <si>
@@ -238,6 +235,30 @@
   </si>
   <si>
     <t>Word Counter displays properly</t>
+  </si>
+  <si>
+    <t>Textarea Changes</t>
+  </si>
+  <si>
+    <t>Test case plan - Day 4 (Final Error Testing and Word Counter)</t>
+  </si>
+  <si>
+    <t>When a note is removed, the remaining notes are reorganized with proper ids set to ensure there are no errors with selecting them for editing or deletion</t>
+  </si>
+  <si>
+    <t>Whenever a function modifies the text input, the wordCount() function is called to update the word counter for new or removed textpad input (i.e. removing notes, displaying a note to edit, etc.)</t>
+  </si>
+  <si>
+    <t>When a note is selected to be edited and it has multiple lines, it is displayed properly in the list with multiple lines displayed</t>
+  </si>
+  <si>
+    <t>When View Notes is clicked while the users notes are already being viewed, an error message will be displayed telling the user they are already viewing their notes</t>
+  </si>
+  <si>
+    <t>When View Notes is clicked with a new username entered while viewing another user's notes, the new username's notes will be displayed</t>
+  </si>
+  <si>
+    <t>When a note is selected to be edited or deleted and the username input is changed, the edit or deletion will occur for the user who owns the note, instead of the new username</t>
   </si>
 </sst>
 </file>
@@ -737,7 +758,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -823,7 +844,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>5</v>
@@ -852,7 +873,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>5</v>
@@ -878,7 +899,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>5</v>
@@ -904,7 +925,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>5</v>
@@ -930,7 +951,7 @@
         <v>23</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>5</v>
@@ -959,7 +980,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>5</v>
@@ -985,7 +1006,7 @@
         <v>24</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>5</v>
@@ -1136,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D38B54-E88D-4CB1-BE10-C352126323F4}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1243,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>5</v>
@@ -1251,7 +1272,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>5</v>
@@ -1277,7 +1298,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>5</v>
@@ -1303,7 +1324,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>5</v>
@@ -1604,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA979D8D-68B0-424C-8427-B4FECE51615E}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1711,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>5</v>
@@ -1719,7 +1740,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>5</v>
@@ -1745,7 +1766,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>5</v>
@@ -1771,7 +1792,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>5</v>
@@ -1797,7 +1818,7 @@
         <v>47</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>5</v>
@@ -1823,7 +1844,7 @@
         <v>48</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>5</v>
@@ -2321,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109493BF-EF21-46D5-86B4-855D12656052}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,7 +2363,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -2400,19 +2421,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>5</v>
@@ -2429,19 +2447,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>5</v>
@@ -2453,7 +2471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2464,10 +2482,13 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>5</v>
@@ -2479,47 +2500,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>5</v>
@@ -2531,7 +2552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -2542,7 +2563,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>12</v>
@@ -2557,7 +2578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -2568,7 +2589,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>12</v>
@@ -2583,7 +2604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -2594,7 +2615,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>12</v>
@@ -2620,7 +2641,7 @@
         <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>12</v>
@@ -2635,7 +2656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2646,10 +2667,7 @@
         <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>12</v>
@@ -2664,7 +2682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2675,34 +2693,37 @@
         <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="F15" s="2" t="s">
         <v>12</v>
       </c>
@@ -2716,7 +2737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -2727,7 +2748,7 @@
         <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>12</v>
@@ -2742,7 +2763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -2753,34 +2774,34 @@
         <v>22</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>15</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="F18" s="2" t="s">
         <v>12</v>
       </c>
@@ -2794,7 +2815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -2805,7 +2826,7 @@
         <v>22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>12</v>
@@ -2820,7 +2841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -2831,7 +2852,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>12</v>
@@ -2846,7 +2867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -2857,7 +2878,7 @@
         <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>12</v>
@@ -2872,7 +2893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -2883,34 +2904,35 @@
         <v>22</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>20</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
         <v>12</v>
       </c>
@@ -2924,20 +2946,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="24" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="E24" s="4"/>
       <c r="F24" s="2" t="s">
         <v>12</v>
       </c>
@@ -2959,10 +2981,10 @@
         <v>40</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
@@ -2989,7 +3011,7 @@
         <v>43</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
@@ -3005,7 +3027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -3016,7 +3038,7 @@
         <v>43</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -3032,34 +3054,213 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>30</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>31</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>